<commit_message>
Arrumando Mapas para o CAP-3
</commit_message>
<xml_diff>
--- a/IEBgeo/IEB-resu.xlsx
+++ b/IEBgeo/IEB-resu.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>ANO</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Par.ss</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>pbias(%)</t>
   </si>
 </sst>
 </file>
@@ -327,12 +333,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:21"/>
+  <dimension ref="1:23"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -502,7 +508,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="8" t="n">
-        <v>-0.058</v>
+        <v>0.5338</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0.5467</v>
@@ -523,7 +529,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="8" t="n">
-        <v>-0.1006</v>
+        <v>-0.058</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>-0.0716</v>
@@ -544,7 +550,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="8" t="n">
-        <v>-0.3145</v>
+        <v>-0.1006</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>-0.1292</v>
@@ -564,7 +570,9 @@
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="8" t="n">
+        <v>-0.3145</v>
+      </c>
       <c r="C12" s="0" t="n">
         <v>-0.288</v>
       </c>
@@ -583,7 +591,6 @@
       <c r="A13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="0" t="n">
         <v>-0.2726</v>
@@ -756,6 +763,46 @@
         <v>6</v>
       </c>
       <c r="G21" s="9"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0.06493221681</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0.06211737423</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0.06867107298</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0.06403996941</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>0.06694027643</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0.1968729675</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>-0.0048426933</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>0.5077838162</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.3517482654</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>0.2019460244</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>